<commit_message>
refactor: migrate from fal.ai to kie.ai API for video generation
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -31,7 +31,7 @@
     <t>status</t>
   </si>
   <si>
-    <t>request_id</t>
+    <t>task_id</t>
   </si>
   <si>
     <t>video_url</t>
@@ -43,28 +43,28 @@
     <t>created_at</t>
   </si>
   <si>
-    <t>Alien comedian mocks humans blindly trusting AI</t>
-  </si>
-  <si>
-    <t>Alien roasts humans trusting AI 🤖🔥 #aliencomedy #aijokes #extraterrestrialhumor #futuretech #funny #viral #memes #lol #trendingnow #comedyvideo #spacehumor #airoast</t>
-  </si>
-  <si>
-    <t>Futuristic comedy club on Mars, neon lights, diverse alien audience, cinematic realism, spotlight on alien comic, holographic AI images flickering behind</t>
-  </si>
-  <si>
-    <t>In a packed futuristic comedy club on Mars, bathed in swirling neon purples and blues, an alien comedian stands under a harsh spotlight on a small stage, their textured green skin shimmering slightly in the light. Behind them, flickering holographic images of various AI interfaces glitch and morph, casting eerie, shifting shadows. The comedian leans in close to the camera, their large eyes gleaming with sly amusement as they deliver a sharp, sardonic line about humans blindly trusting AI without question, voice dripping with ironic humor. They smirk knowingly and slowly pan the camera across the diverse crowd of aliens—tentacles, scales, and eyes of all shapes—who chuckle and whisper among themselves. The lens is a wide-angle 24mm with a subtle grainy film stock that captures every neon reflection and shadow detail, lending a raw, documentary feel to the selfie shot. Ambient sounds include murmurs of alien laughter, the soft hum of the holograms, and faint clinking of glasses. Behind the character, the vibrant club’s neon signs pulse softly against the dark Martian sky visible through the windowed walls. - **Main character:** green-skinned alien comedian with textured skin and expressive large eyes - **They say:** “You humans just hand your brains over to AI like it’s a cosmic joke—and guess what? We’re the punchline.” - **They** smirk slyly and pan the camera slowly across the amused alien audience. - **Time of Day:** night - **Lens:** wide-angle 24mm with grainy film stock - **Audio:** alien laughter, hologram hums, clinking glasses - **Background:** neon-lit futuristic comedy club interior with flickering AI holograms and a diverse alien crowd visible behind.</t>
-  </si>
-  <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t>7a6836f4-e187-4577-94e1-3d59a93d42c6</t>
-  </si>
-  <si>
-    <t>https://v3.fal.media/files/kangaroo/sHJaLBGQgqYjkJg518fZ-_output.mp4</t>
-  </si>
-  <si>
-    <t>2025-06-22 20:07</t>
+    <t>Meteorologist woman narrowly escapes tornado while reporting live</t>
+  </si>
+  <si>
+    <t>Tornado chase live: meteorologist’s heart-stopping twist! 🌪️ #weatherwatch #stormchasing #tornadoalert #meteorology #viral #trending #livebroadcast #breakingnews #stormseason #extremeweather #newsflash #onair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open plains with dark swirling clouds, tornado funnel forming, meteorologist running with camera crew, cinematic realism, dynamic wind effects, intense sky contrast, emergency vehicles in background, handheld docu-style shot, suspenseful atmosphere, dust and debris flying around, lightning flashes intermittently in the stormy sky, dramatic close-ups on the meteorologist’s determined face, vivid weather phenomena dominating the scene, wide shots capturing the scale of the tornado and the chaos it causes, real-time live broadcast graphics overlayed on screen, urgency and tension palpable in the air, natural sounds of wind howling mixed with urgent voiceover, gritty realism with high-definition clarity, emotionally charged and immersive visual experience, blending raw nature power and human bravery, cinematic color grading emphasizing the storm’s ominous hues, fast-paced editing capturing every moment of the chase, immersive audio capturing the roar of the tornado and meteorologist’s breathless commentary.  </t>
+  </si>
+  <si>
+    <t>A woman with wind-tossed hair and a soaked jacket holds a handheld camera close, her face streaked with rain and dirt as a massive tornado funnel spirals ominously behind her across the flat, open plains. She gasps into the mic, voice tight with adrenaline, “This thing’s coming faster than we thought—everyone, get clear, now!” The frame jitters as she stumbles forward, the camera shaking from her hurried steps and the howling wind that whips dust and debris past the lens. Lightning flashes illuminate the angry sky, casting sharp shadows on her determined expression as emergency vehicles flash red and blue lights in the distance. The shot is tight, selfie-style with a wide-angle lens that captures the swirling clouds pressing down and the tornado’s terrifying scale, filmed on high-definition stock with gritty, cinematic color grading emphasizing dark stormy blues and ominous grays. The relentless roar of the storm mingles with her breathless voiceover, the chaotic energy palpable as she glances nervously over her shoulder while pressing forward against the gale. Time of Day: late afternoon dusk. Lens: wide-angle handheld, high-definition stock. Audio: howling wind, crackling thunder, distant sirens. Background: swirling storm clouds, tornado funnel, emergency vehicles racing across the plains behind her.</t>
+  </si>
+  <si>
+    <t>in_progress</t>
+  </si>
+  <si>
+    <t>e4e5cbd3f1c65f6aeeaa8b4bdb74ba00</t>
+  </si>
+  <si>
+    <t>https://tempfile.aiquickdraw.com/p/a78a5a1538a444519c4b12d87c9c2bed_1752142446.mp4</t>
+  </si>
+  <si>
+    <t>2025-07-10 12:10</t>
   </si>
 </sst>
 </file>
@@ -82,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>

</xml_diff>